<commit_message>
[ excel automation ] openpyxl atomation employees project example
</commit_message>
<xml_diff>
--- a/_04_excel_automation/generated/employees.xlsx
+++ b/_04_excel_automation/generated/employees.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Kitty" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Maeva" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Gertude" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,24 +415,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -443,14 +426,66 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>hello</t>
+          <t>Maeva</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>world</t>
+          <t>Gertude</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello Maeva!</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello Gertude!</t>
         </is>
       </c>
     </row>

</xml_diff>